<commit_message>
themed graphs, split categories with label wrap
</commit_message>
<xml_diff>
--- a/tidy data for vada-upa experiment2.xlsx
+++ b/tidy data for vada-upa experiment2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umhealth-my.sharepoint.com/personal/yongfeng_med_umich_edu/Documents/Desktop/VADA UPA project/vada upd exp2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/peterhiggins/Documents/RCode/upa_vada_mice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2099C9B0-0E1D-4DF7-87F3-9F2C4AA088E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22D8393D-486F-B14B-926F-E74F1018E258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{9636FDD7-7000-4F9F-B7D1-9703FCCB722F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19440" windowHeight="14880" xr2:uid="{9636FDD7-7000-4F9F-B7D1-9703FCCB722F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,26 +74,26 @@
     <t>day7 stool bleeding</t>
   </si>
   <si>
-    <t>water+vehicle</t>
+    <t>DSS+  vehicle</t>
   </si>
   <si>
-    <t>water+Vada/Upa</t>
+    <t>DSS+  Vada/Upa</t>
   </si>
   <si>
-    <t>DSS+vehicle</t>
+    <t>DSS+  Upa</t>
   </si>
   <si>
-    <t>DSS+Vada/Upa</t>
+    <t>water+ vehicle</t>
   </si>
   <si>
-    <t>DSS+Upa</t>
+    <t>water+ Vada/Upa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -906,22 +906,22 @@
   <dimension ref="A1:L46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="C6" sqref="C6:C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.1640625" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -959,7 +959,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="5">
         <v>836</v>
       </c>
@@ -967,7 +967,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D2" s="6">
         <v>21.894736842105264</v>
@@ -997,7 +997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>837</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4">
         <v>20.526315789473685</v>
@@ -1035,7 +1035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>839</v>
       </c>
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D4" s="4">
         <v>24.26829268292683</v>
@@ -1073,7 +1073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>841</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D5" s="13">
         <v>23.25</v>
@@ -1111,7 +1111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="15">
         <v>831</v>
       </c>
@@ -1119,7 +1119,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D6" s="16">
         <v>22.631578947368421</v>
@@ -1149,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="18">
         <v>832</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4">
         <v>20.365853658536587</v>
@@ -1187,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
         <v>833</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D8" s="4">
         <v>24.390243902439025</v>
@@ -1225,7 +1225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="18">
         <v>859</v>
       </c>
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D9" s="4">
         <v>22.375</v>
@@ -1263,7 +1263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>860</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D10" s="13">
         <v>23.625</v>
@@ -1301,7 +1301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="21">
         <v>861</v>
       </c>
@@ -1309,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="6">
         <v>33.333333333333336</v>
@@ -1339,7 +1339,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>862</v>
       </c>
@@ -1347,7 +1347,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D12" s="4">
         <v>27.285714285714285</v>
@@ -1377,7 +1377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="23">
         <v>863</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D13" s="4">
         <v>27.666666666666668</v>
@@ -1415,7 +1415,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="23">
         <v>874</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D14" s="4">
         <v>42</v>
@@ -1453,7 +1453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="23">
         <v>865</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D15" s="4">
         <v>34.406779661016948</v>
@@ -1491,7 +1491,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="26">
         <v>866</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D16" s="4">
         <v>34.666666666666664</v>
@@ -1529,7 +1529,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="26">
         <v>867</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" s="4">
         <v>32.909090909090907</v>
@@ -1567,7 +1567,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="26">
         <v>868</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D18" s="4">
         <v>29.310344827586206</v>
@@ -1605,7 +1605,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="26">
         <v>869</v>
       </c>
@@ -1613,7 +1613,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D19" s="4">
         <v>34.736842105263158</v>
@@ -1643,7 +1643,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="27">
         <v>870</v>
       </c>
@@ -1651,7 +1651,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D20" s="13">
         <v>33.846153846153847</v>
@@ -1681,7 +1681,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="29">
         <v>851</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D21" s="6">
         <v>17.571428571428573</v>
@@ -1719,7 +1719,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="32">
         <v>852</v>
       </c>
@@ -1727,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D22" s="4">
         <v>25.875</v>
@@ -1757,7 +1757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="32">
         <v>853</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>4</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D23" s="4">
         <v>22.133333333333333</v>
@@ -1795,7 +1795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="32">
         <v>854</v>
       </c>
@@ -1803,7 +1803,7 @@
         <v>4</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D24" s="4">
         <v>24.153846153846153</v>
@@ -1833,7 +1833,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="32">
         <v>855</v>
       </c>
@@ -1841,7 +1841,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D25" s="4">
         <v>22.571428571428573</v>
@@ -1871,7 +1871,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="34">
         <v>826</v>
       </c>
@@ -1879,7 +1879,7 @@
         <v>4</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D26" s="4">
         <v>26</v>
@@ -1909,7 +1909,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="34">
         <v>827</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>4</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D27" s="4">
         <v>24.428571428571427</v>
@@ -1947,7 +1947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="34">
         <v>828</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>4</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D28" s="4">
         <v>31.93548387096774</v>
@@ -1985,7 +1985,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="34">
         <v>829</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D29" s="4">
         <v>20</v>
@@ -2023,7 +2023,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="37">
         <v>830</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D30" s="13">
         <v>25</v>
@@ -2061,7 +2061,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="39">
         <v>871</v>
       </c>
@@ -2069,7 +2069,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D31" s="6">
         <v>26.176470588235293</v>
@@ -2099,7 +2099,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="41">
         <v>872</v>
       </c>
@@ -2107,7 +2107,7 @@
         <v>5</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D32" s="4">
         <v>26.833333333333332</v>
@@ -2137,7 +2137,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="41">
         <v>873</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>5</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D33" s="4">
         <v>35</v>
@@ -2175,7 +2175,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="41">
         <v>840</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>5</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D34" s="4">
         <v>31.692307692307693</v>
@@ -2213,7 +2213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="41">
         <v>641</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>5</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D35" s="4">
         <v>26</v>
@@ -2251,7 +2251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="42">
         <v>856</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>5</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D36" s="4">
         <v>30.428571428571427</v>
@@ -2287,7 +2287,7 @@
       </c>
       <c r="L36" s="25"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="42">
         <v>857</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>5</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D37" s="4">
         <v>28.333333333333332</v>
@@ -2325,7 +2325,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="42">
         <v>858</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>5</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D38" s="4">
         <v>31.692307692307693</v>
@@ -2363,7 +2363,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="42">
         <v>834</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D39" s="4">
         <v>36.727272727272727</v>
@@ -2401,7 +2401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="43">
         <v>835</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>5</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D40" s="13">
         <v>21.666666666666668</v>
@@ -2439,7 +2439,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="45"/>
       <c r="B42" s="46"/>
       <c r="C42" s="46"/>
@@ -2447,7 +2447,7 @@
       <c r="E42" s="46"/>
       <c r="F42" s="46"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="45"/>
       <c r="B43" s="46"/>
       <c r="C43" s="46"/>
@@ -2455,7 +2455,7 @@
       <c r="E43" s="46"/>
       <c r="F43" s="46"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="45"/>
       <c r="B44" s="46"/>
       <c r="C44" s="46"/>
@@ -2463,7 +2463,7 @@
       <c r="E44" s="46"/>
       <c r="F44" s="46"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="45"/>
       <c r="B45" s="47"/>
       <c r="C45" s="48"/>
@@ -2471,7 +2471,7 @@
       <c r="E45" s="48"/>
       <c r="F45" s="49"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="45"/>
       <c r="B46" s="47"/>
       <c r="C46" s="48"/>

</xml_diff>